<commit_message>
getting peak times of high flow events
</commit_message>
<xml_diff>
--- a/Suspended_Sediment_Analysis/LANL_SS/down_LANL.xlsx
+++ b/Suspended_Sediment_Analysis/LANL_SS/down_LANL.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,15 +8,28 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\huck4481\Documents\GitHub\La_Jara\Suspended_Sediment_Analysis\LANL_SS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{906DA7E7-0DE3-4FA8-B852-2744F48C3DE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28D719BF-813F-4B6D-BCD1-7B6BC5BFDA05}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-25320" yWindow="195" windowWidth="25440" windowHeight="15390" activeTab="1"/>
+    <workbookView minimized="1" xWindow="-24705" yWindow="570" windowWidth="22260" windowHeight="14940" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Chart1" sheetId="2" r:id="rId1"/>
     <sheet name="down_LANL" sheetId="1" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -35,7 +48,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -6305,7 +6318,7 @@
 </file>
 
 <file path=xl/chartsheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr/>
   <sheetViews>
     <sheetView zoomScale="112" workbookViewId="0" zoomToFit="1"/>
@@ -6763,11 +6776,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E101"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O14" sqref="O14"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="O36" sqref="O36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
prepping SS vs TURB relation plots for USGS meeting
</commit_message>
<xml_diff>
--- a/Suspended_Sediment_Analysis/LANL_SS/down_LANL.xlsx
+++ b/Suspended_Sediment_Analysis/LANL_SS/down_LANL.xlsx
@@ -8,13 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\huck4481\Documents\GitHub\La_Jara\Suspended_Sediment_Analysis\LANL_SS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28D719BF-813F-4B6D-BCD1-7B6BC5BFDA05}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BCD8660-E820-4277-B817-8830D04D6AC9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="-24705" yWindow="570" windowWidth="22260" windowHeight="14940" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-25320" yWindow="195" windowWidth="25440" windowHeight="15390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Chart1" sheetId="2" r:id="rId1"/>
-    <sheet name="down_LANL" sheetId="1" r:id="rId2"/>
+    <sheet name="down_LANL" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -604,901 +603,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:layout/>
-      <c:barChart>
-        <c:barDir val="col"/>
-        <c:grouping val="clustered"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent1"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:val>
-            <c:numRef>
-              <c:f>down_LANL!$B$2:$B$101</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="100"/>
-                <c:pt idx="0">
-                  <c:v>21.59</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>19.968</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>10.484</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>13.013999999999999</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>9.6660000000000004</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>9.15133333333333</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>7.6153333333333304</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>4.4593333333333298</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>5.7193333333333296</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>10.9166666666666</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>14.478</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>22.442</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>13.925999999999901</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>9.5079999999999991</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>7.5993333333333304</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>6.7193333333333296</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>6.1219999999999999</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>3.4268419502040599</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>3.4224692347058099</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>3.4180965192075599</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>3.4137238037093098</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>3.40060565721457</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>3.39623294171632</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>3.3874875107198301</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>3.3831147952215801</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>3.3787420797233301</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>4.5357048000000004</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>12.730442</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>12.263458</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>10.282138</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>13.492993999999999</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>11.935922</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>11.653563999999999</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>10.448041999999999</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>10.018212</c:v>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v>8.6619565999999999</c:v>
-                </c:pt>
-                <c:pt idx="36">
-                  <c:v>8.1737145112</c:v>
-                </c:pt>
-                <c:pt idx="37">
-                  <c:v>9.4050313999999897</c:v>
-                </c:pt>
-                <c:pt idx="38">
-                  <c:v>9.9722711999999998</c:v>
-                </c:pt>
-                <c:pt idx="39">
-                  <c:v>6.2565413999999997</c:v>
-                </c:pt>
-                <c:pt idx="40">
-                  <c:v>6.1596501999999997</c:v>
-                </c:pt>
-                <c:pt idx="41">
-                  <c:v>6.5126184</c:v>
-                </c:pt>
-                <c:pt idx="42">
-                  <c:v>12.555218</c:v>
-                </c:pt>
-                <c:pt idx="43">
-                  <c:v>10.2862428</c:v>
-                </c:pt>
-                <c:pt idx="44">
-                  <c:v>8.4326103999999997</c:v>
-                </c:pt>
-                <c:pt idx="45">
-                  <c:v>8.0923947999999992</c:v>
-                </c:pt>
-                <c:pt idx="46">
-                  <c:v>7.7965476000000002</c:v>
-                </c:pt>
-                <c:pt idx="47">
-                  <c:v>6.1084097999999996</c:v>
-                </c:pt>
-                <c:pt idx="48">
-                  <c:v>6.5571175999999998</c:v>
-                </c:pt>
-                <c:pt idx="49">
-                  <c:v>6.4697841999999897</c:v>
-                </c:pt>
-                <c:pt idx="50">
-                  <c:v>6.5095738000000001</c:v>
-                </c:pt>
-                <c:pt idx="51">
-                  <c:v>5.9067411999999999</c:v>
-                </c:pt>
-                <c:pt idx="52">
-                  <c:v>8.6772618000000001</c:v>
-                </c:pt>
-                <c:pt idx="53">
-                  <c:v>9.5304336000000003</c:v>
-                </c:pt>
-                <c:pt idx="54">
-                  <c:v>7.8862117999999999</c:v>
-                </c:pt>
-                <c:pt idx="55">
-                  <c:v>7.5004643999999896</c:v>
-                </c:pt>
-                <c:pt idx="56">
-                  <c:v>9.4601454</c:v>
-                </c:pt>
-                <c:pt idx="57">
-                  <c:v>6.7386191999999996</c:v>
-                </c:pt>
-                <c:pt idx="58">
-                  <c:v>9.4574637999999993</c:v>
-                </c:pt>
-                <c:pt idx="59">
-                  <c:v>4.3573475999999998</c:v>
-                </c:pt>
-                <c:pt idx="60">
-                  <c:v>6.9575446000000003</c:v>
-                </c:pt>
-                <c:pt idx="61">
-                  <c:v>6.2245963151999897</c:v>
-                </c:pt>
-                <c:pt idx="62">
-                  <c:v>9.6673880440000008</c:v>
-                </c:pt>
-                <c:pt idx="63">
-                  <c:v>11.6311664</c:v>
-                </c:pt>
-                <c:pt idx="64">
-                  <c:v>5.0034375635999897</c:v>
-                </c:pt>
-                <c:pt idx="66">
-                  <c:v>18.038439999999898</c:v>
-                </c:pt>
-                <c:pt idx="67">
-                  <c:v>11.934466</c:v>
-                </c:pt>
-                <c:pt idx="68">
-                  <c:v>10.379066</c:v>
-                </c:pt>
-                <c:pt idx="69">
-                  <c:v>13.443178</c:v>
-                </c:pt>
-                <c:pt idx="70">
-                  <c:v>24.053342000000001</c:v>
-                </c:pt>
-                <c:pt idx="71">
-                  <c:v>13.279764</c:v>
-                </c:pt>
-                <c:pt idx="72">
-                  <c:v>8.0217293999999999</c:v>
-                </c:pt>
-                <c:pt idx="73">
-                  <c:v>10.49208</c:v>
-                </c:pt>
-                <c:pt idx="74">
-                  <c:v>8.7961375999999998</c:v>
-                </c:pt>
-                <c:pt idx="75">
-                  <c:v>6.6968831999999896</c:v>
-                </c:pt>
-                <c:pt idx="76">
-                  <c:v>10.1770552</c:v>
-                </c:pt>
-                <c:pt idx="77">
-                  <c:v>18.713209200000001</c:v>
-                </c:pt>
-                <c:pt idx="78">
-                  <c:v>13.83131</c:v>
-                </c:pt>
-                <c:pt idx="79">
-                  <c:v>13.83131</c:v>
-                </c:pt>
-                <c:pt idx="80">
-                  <c:v>10.596176</c:v>
-                </c:pt>
-                <c:pt idx="81">
-                  <c:v>20.1574232</c:v>
-                </c:pt>
-                <c:pt idx="82">
-                  <c:v>31.815999999999999</c:v>
-                </c:pt>
-                <c:pt idx="83">
-                  <c:v>36.380000000000003</c:v>
-                </c:pt>
-                <c:pt idx="84">
-                  <c:v>34.868000000000002</c:v>
-                </c:pt>
-                <c:pt idx="85">
-                  <c:v>33.26</c:v>
-                </c:pt>
-                <c:pt idx="86">
-                  <c:v>26.347999999999999</c:v>
-                </c:pt>
-                <c:pt idx="87">
-                  <c:v>20.135999999999999</c:v>
-                </c:pt>
-                <c:pt idx="88">
-                  <c:v>16.759999999999899</c:v>
-                </c:pt>
-                <c:pt idx="89">
-                  <c:v>22.84</c:v>
-                </c:pt>
-                <c:pt idx="90">
-                  <c:v>15.56</c:v>
-                </c:pt>
-                <c:pt idx="91">
-                  <c:v>13.776</c:v>
-                </c:pt>
-                <c:pt idx="92">
-                  <c:v>11.31</c:v>
-                </c:pt>
-                <c:pt idx="93">
-                  <c:v>8.7560000000000002</c:v>
-                </c:pt>
-                <c:pt idx="94">
-                  <c:v>1.6175579133510101</c:v>
-                </c:pt>
-                <c:pt idx="95">
-                  <c:v>1.6136321839080401</c:v>
-                </c:pt>
-                <c:pt idx="96">
-                  <c:v>1.6097064544650701</c:v>
-                </c:pt>
-                <c:pt idx="97">
-                  <c:v>1.6057807250220999</c:v>
-                </c:pt>
-                <c:pt idx="98">
-                  <c:v>1.6018549955791299</c:v>
-                </c:pt>
-                <c:pt idx="99">
-                  <c:v>1.5974058355437599</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-57C1-4B41-A9AE-5C79FEA55C11}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent2"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:val>
-            <c:numRef>
-              <c:f>down_LANL!$C$2:$C$101</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="100"/>
-                <c:pt idx="0">
-                  <c:v>57.73</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>48.06</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>17.43</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>11.45</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>55</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>6.53</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>45.16</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>8.48</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>10.74</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>19.84</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>49.09</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>35.39</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>23.68</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>9.89</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>4.08</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>1.65</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>0.84</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>12.38</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>9.4700000000000006</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>10.48</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>9.33</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>9.66</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>1.5</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>5.5</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>8.9499999999999993</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>9.5</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>4.5</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>15</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>10</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>6.82</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>3.5</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v>6.25</c:v>
-                </c:pt>
-                <c:pt idx="36">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="37">
-                  <c:v>10.34</c:v>
-                </c:pt>
-                <c:pt idx="38">
-                  <c:v>5.33</c:v>
-                </c:pt>
-                <c:pt idx="39">
-                  <c:v>6.43</c:v>
-                </c:pt>
-                <c:pt idx="40">
-                  <c:v>6.43</c:v>
-                </c:pt>
-                <c:pt idx="41">
-                  <c:v>14.19</c:v>
-                </c:pt>
-                <c:pt idx="42">
-                  <c:v>14.74</c:v>
-                </c:pt>
-                <c:pt idx="43">
-                  <c:v>18.95</c:v>
-                </c:pt>
-                <c:pt idx="44">
-                  <c:v>26.09</c:v>
-                </c:pt>
-                <c:pt idx="45">
-                  <c:v>7.27</c:v>
-                </c:pt>
-                <c:pt idx="46">
-                  <c:v>5.33</c:v>
-                </c:pt>
-                <c:pt idx="47">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="48">
-                  <c:v>12.14</c:v>
-                </c:pt>
-                <c:pt idx="49">
-                  <c:v>10.67</c:v>
-                </c:pt>
-                <c:pt idx="50">
-                  <c:v>5.29</c:v>
-                </c:pt>
-                <c:pt idx="51">
-                  <c:v>4.12</c:v>
-                </c:pt>
-                <c:pt idx="52">
-                  <c:v>8.1300000000000008</c:v>
-                </c:pt>
-                <c:pt idx="53">
-                  <c:v>6.88</c:v>
-                </c:pt>
-                <c:pt idx="54">
-                  <c:v>4.83</c:v>
-                </c:pt>
-                <c:pt idx="55">
-                  <c:v>2.35</c:v>
-                </c:pt>
-                <c:pt idx="56">
-                  <c:v>5.33</c:v>
-                </c:pt>
-                <c:pt idx="57">
-                  <c:v>5.29</c:v>
-                </c:pt>
-                <c:pt idx="58">
-                  <c:v>3.23</c:v>
-                </c:pt>
-                <c:pt idx="59">
-                  <c:v>3.33</c:v>
-                </c:pt>
-                <c:pt idx="60">
-                  <c:v>5.33</c:v>
-                </c:pt>
-                <c:pt idx="61">
-                  <c:v>10.67</c:v>
-                </c:pt>
-                <c:pt idx="62">
-                  <c:v>7.86</c:v>
-                </c:pt>
-                <c:pt idx="63">
-                  <c:v>8.67</c:v>
-                </c:pt>
-                <c:pt idx="64">
-                  <c:v>9.3800000000000008</c:v>
-                </c:pt>
-                <c:pt idx="66">
-                  <c:v>17.420000000000002</c:v>
-                </c:pt>
-                <c:pt idx="67">
-                  <c:v>6.67</c:v>
-                </c:pt>
-                <c:pt idx="68">
-                  <c:v>2.5</c:v>
-                </c:pt>
-                <c:pt idx="69">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="70">
-                  <c:v>22.14</c:v>
-                </c:pt>
-                <c:pt idx="71">
-                  <c:v>10</c:v>
-                </c:pt>
-                <c:pt idx="72">
-                  <c:v>6.43</c:v>
-                </c:pt>
-                <c:pt idx="73">
-                  <c:v>18</c:v>
-                </c:pt>
-                <c:pt idx="74">
-                  <c:v>9.33</c:v>
-                </c:pt>
-                <c:pt idx="75">
-                  <c:v>5.71</c:v>
-                </c:pt>
-                <c:pt idx="76">
-                  <c:v>2.86</c:v>
-                </c:pt>
-                <c:pt idx="77">
-                  <c:v>20.67</c:v>
-                </c:pt>
-                <c:pt idx="78">
-                  <c:v>4.67</c:v>
-                </c:pt>
-                <c:pt idx="79">
-                  <c:v>11.88</c:v>
-                </c:pt>
-                <c:pt idx="80">
-                  <c:v>2.86</c:v>
-                </c:pt>
-                <c:pt idx="81">
-                  <c:v>8.75</c:v>
-                </c:pt>
-                <c:pt idx="83">
-                  <c:v>110</c:v>
-                </c:pt>
-                <c:pt idx="84">
-                  <c:v>53.33</c:v>
-                </c:pt>
-                <c:pt idx="85">
-                  <c:v>80</c:v>
-                </c:pt>
-                <c:pt idx="86">
-                  <c:v>43.33</c:v>
-                </c:pt>
-                <c:pt idx="87">
-                  <c:v>92.22</c:v>
-                </c:pt>
-                <c:pt idx="88">
-                  <c:v>52.22</c:v>
-                </c:pt>
-                <c:pt idx="89">
-                  <c:v>76.150000000000006</c:v>
-                </c:pt>
-                <c:pt idx="90">
-                  <c:v>41.2</c:v>
-                </c:pt>
-                <c:pt idx="91">
-                  <c:v>39.6</c:v>
-                </c:pt>
-                <c:pt idx="92">
-                  <c:v>27.6</c:v>
-                </c:pt>
-                <c:pt idx="93">
-                  <c:v>20.83</c:v>
-                </c:pt>
-                <c:pt idx="94">
-                  <c:v>37.6</c:v>
-                </c:pt>
-                <c:pt idx="95">
-                  <c:v>31.54</c:v>
-                </c:pt>
-                <c:pt idx="96">
-                  <c:v>28.08</c:v>
-                </c:pt>
-                <c:pt idx="97">
-                  <c:v>23.6</c:v>
-                </c:pt>
-                <c:pt idx="98">
-                  <c:v>21.18</c:v>
-                </c:pt>
-                <c:pt idx="99">
-                  <c:v>23.14</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-57C1-4B41-A9AE-5C79FEA55C11}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:gapWidth val="219"/>
-        <c:overlap val="-27"/>
-        <c:axId val="1919564576"/>
-        <c:axId val="1924350128"/>
-      </c:barChart>
-      <c:catAx>
-        <c:axId val="1919564576"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="15000"/>
-                <a:lumOff val="85000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="1924350128"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="1924350128"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln>
-            <a:noFill/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="1919564576"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
-      </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-    </c:plotArea>
-    <c:legend>
-      <c:legendPos val="b"/>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:legend>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:extLst>
-      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
-        <c16r3:dataDisplayOptions16>
-          <c16r3:dispNaAsBlank val="1"/>
-        </c16r3:dataDisplayOptions16>
-      </c:ext>
-    </c:extLst>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:schemeClr val="bg1"/>
-    </a:solidFill>
-    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:round/>
-    </a:ln>
-    <a:effectLst/>
-  </c:spPr>
-  <c:txPr>
-    <a:bodyPr/>
-    <a:lstStyle/>
-    <a:p>
-      <a:pPr>
-        <a:defRPr/>
-      </a:pPr>
-      <a:endParaRPr lang="en-US"/>
-    </a:p>
-  </c:txPr>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-  <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:title>
       <c:tx>
         <c:rich>
           <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
@@ -2552,7 +1656,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -3521,7 +2625,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -4226,48 +3330,8 @@
 </cs:colorStyle>
 </file>
 
-<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
-  <a:schemeClr val="accent1"/>
-  <a:schemeClr val="accent2"/>
-  <a:schemeClr val="accent3"/>
-  <a:schemeClr val="accent4"/>
-  <a:schemeClr val="accent5"/>
-  <a:schemeClr val="accent6"/>
-  <cs:variation/>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-    <a:lumOff val="20000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-    <a:lumOff val="40000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-    <a:lumOff val="30000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-    <a:lumOff val="50000"/>
-  </cs:variation>
-</cs:colorStyle>
-</file>
-
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
@@ -4294,8 +3358,8 @@
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -4396,7 +3460,7 @@
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="28575" cap="rnd">
+      <a:ln w="19050" cap="rnd">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
@@ -4428,10 +3492,10 @@
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="rnd">
@@ -4471,22 +3535,23 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
         <a:schemeClr val="dk1">
-          <a:lumMod val="65000"/>
-          <a:lumOff val="35000"/>
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
         </a:schemeClr>
       </a:solidFill>
-      <a:ln w="9525">
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
             <a:lumMod val="65000"/>
             <a:lumOff val="35000"/>
           </a:schemeClr>
         </a:solidFill>
+        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:downBar>
@@ -4591,8 +3656,8 @@
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="75000"/>
-            <a:lumOff val="25000"/>
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -4724,19 +3789,20 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
         <a:schemeClr val="lt1"/>
       </a:solidFill>
-      <a:ln w="9525">
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
           </a:schemeClr>
         </a:solidFill>
+        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:upBar>
@@ -4750,6 +3816,17 @@
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:valueAxis>
   <cs:wall>
@@ -5801,580 +4878,20 @@
 </cs:chartStyle>
 </file>
 
-<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
-  <cs:axisTitle>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:axisTitle>
-  <cs:categoryAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:categoryAxis>
-  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="bg1"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:chartArea>
-  <cs:dataLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="75000"/>
-        <a:lumOff val="25000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataLabel>
-  <cs:dataLabelCallout>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln>
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
-      <a:spAutoFit/>
-    </cs:bodyPr>
-  </cs:dataLabelCallout>
-  <cs:dataPoint>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:dataPoint>
-  <cs:dataPoint3D>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:dataPoint3D>
-  <cs:dataPointLine>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="19050" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointLine>
-  <cs:dataPointMarker>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
-  <cs:dataPointWireframe>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointWireframe>
-  <cs:dataTable>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataTable>
-  <cs:downBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="dk1">
-          <a:lumMod val="75000"/>
-          <a:lumOff val="25000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:downBar>
-  <cs:dropLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dropLine>
-  <cs:errorBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:errorBar>
-  <cs:floor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:floor>
-  <cs:gridlineMajor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMajor>
-  <cs:gridlineMinor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="5000"/>
-            <a:lumOff val="95000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMinor>
-  <cs:hiLoLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="50000"/>
-            <a:lumOff val="50000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:hiLoLine>
-  <cs:leaderLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:leaderLine>
-  <cs:legend>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:legend>
-  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea>
-  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea3D>
-  <cs:seriesAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:seriesAxis>
-  <cs:seriesLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:seriesLine>
-  <cs:title>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
-  </cs:title>
-  <cs:trendline>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="19050" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:prstDash val="sysDot"/>
-      </a:ln>
-    </cs:spPr>
-  </cs:trendline>
-  <cs:trendlineLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:trendlineLabel>
-  <cs:upBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:upBar>
-  <cs:valueAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:valueAxis>
-  <cs:wall>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:wall>
-</cs:chartStyle>
-</file>
-
-<file path=xl/chartsheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <sheetPr/>
-  <sheetViews>
-    <sheetView zoomScale="112" workbookViewId="0" zoomToFit="1"/>
-  </sheetViews>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
-</chartsheet>
-</file>
-
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:absoluteAnchor>
-    <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="8657545" cy="6284799"/>
-    <xdr:graphicFrame macro="">
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F4EE5D34-570E-5FE9-302A-DB01A8CD48FB}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvGraphicFramePr>
-          <a:graphicFrameLocks noGrp="1"/>
-        </xdr:cNvGraphicFramePr>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:absoluteAnchor>
-</xdr:wsDr>
-</file>
-
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>581025</xdr:colOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>209550</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>28575</xdr:rowOff>
+      <xdr:rowOff>9525</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>276225</xdr:colOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>514350</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>104775</xdr:rowOff>
+      <xdr:rowOff>85725</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -6403,16 +4920,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>581025</xdr:colOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>209550</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>180975</xdr:rowOff>
+      <xdr:rowOff>161925</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>276225</xdr:colOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>514350</xdr:colOff>
       <xdr:row>30</xdr:row>
-      <xdr:rowOff>66675</xdr:rowOff>
+      <xdr:rowOff>47625</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -6441,16 +4958,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>238125</xdr:colOff>
       <xdr:row>30</xdr:row>
-      <xdr:rowOff>142875</xdr:rowOff>
+      <xdr:rowOff>123825</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>304800</xdr:colOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>542925</xdr:colOff>
       <xdr:row>45</xdr:row>
-      <xdr:rowOff>28575</xdr:rowOff>
+      <xdr:rowOff>9525</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -6777,10 +5294,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:E101"/>
+  <dimension ref="A1:D101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="O36" sqref="O36"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="R1" sqref="R1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6964,7 +5481,7 @@
         <v>4.08</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>44781.727777777778</v>
       </c>
@@ -6975,7 +5492,7 @@
         <v>1.65</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>44781.748611111114</v>
       </c>
@@ -6986,7 +5503,7 @@
         <v>0.84</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>45031.520833333336</v>
       </c>
@@ -6996,8 +5513,11 @@
       <c r="C19">
         <v>12.38</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D19">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>45031.6875</v>
       </c>
@@ -7007,8 +5527,11 @@
       <c r="C20">
         <v>9.4700000000000006</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D20">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>45031.854166666664</v>
       </c>
@@ -7018,8 +5541,11 @@
       <c r="C21">
         <v>5</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D21">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>45032.020833333336</v>
       </c>
@@ -7029,8 +5555,11 @@
       <c r="C22">
         <v>4</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D22">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>45032.520833333336</v>
       </c>
@@ -7040,8 +5569,11 @@
       <c r="C23">
         <v>10.48</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D23">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>45032.6875</v>
       </c>
@@ -7051,8 +5583,11 @@
       <c r="C24">
         <v>9.33</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D24">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>45033.020833333336</v>
       </c>
@@ -7062,8 +5597,11 @@
       <c r="C25">
         <v>9.66</v>
       </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>45033.1875</v>
       </c>
@@ -7073,8 +5611,11 @@
       <c r="C26">
         <v>4</v>
       </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D26">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>45033.354166666664</v>
       </c>
@@ -7084,8 +5625,11 @@
       <c r="C27">
         <v>1.5</v>
       </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D27">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>45033.520833333336</v>
       </c>
@@ -7095,8 +5639,11 @@
       <c r="C28">
         <v>5.5</v>
       </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D28">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>45034.020833333336</v>
       </c>
@@ -7106,8 +5653,11 @@
       <c r="C29">
         <v>8.9499999999999993</v>
       </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D29">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>45034.1875</v>
       </c>
@@ -7117,8 +5667,11 @@
       <c r="C30">
         <v>9.5</v>
       </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D30">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>45034.354166666664</v>
       </c>
@@ -7128,8 +5681,11 @@
       <c r="C31">
         <v>4.5</v>
       </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D31">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>45034.895833333336</v>
       </c>
@@ -7139,8 +5695,11 @@
       <c r="C32">
         <v>15</v>
       </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D32">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <v>45035.104166666664</v>
       </c>
@@ -7150,8 +5709,11 @@
       <c r="C33">
         <v>10</v>
       </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D33">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
         <v>45035.3125</v>
       </c>
@@ -7161,8 +5723,11 @@
       <c r="C34">
         <v>6.82</v>
       </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D34">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
         <v>45035.520833333336</v>
       </c>
@@ -7172,8 +5737,11 @@
       <c r="C35">
         <v>3.5</v>
       </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D35">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
         <v>45036.770833333336</v>
       </c>
@@ -7183,8 +5751,11 @@
       <c r="C36">
         <v>6</v>
       </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D36">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
         <v>45036.979166666664</v>
       </c>
@@ -7194,8 +5765,11 @@
       <c r="C37">
         <v>6.25</v>
       </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D37">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
         <v>45037.1875</v>
       </c>
@@ -7205,8 +5779,11 @@
       <c r="C38">
         <v>6</v>
       </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D38">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
         <v>45039.666666666664</v>
       </c>
@@ -7216,8 +5793,11 @@
       <c r="C39">
         <v>10.34</v>
       </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D39">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
         <v>45039.875</v>
       </c>
@@ -7227,8 +5807,11 @@
       <c r="C40">
         <v>5.33</v>
       </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D40">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
         <v>45040.083333333336</v>
       </c>
@@ -7238,8 +5821,11 @@
       <c r="C41">
         <v>6.43</v>
       </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D41">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
         <v>45040.291666666664</v>
       </c>
@@ -7249,8 +5835,11 @@
       <c r="C42">
         <v>6.43</v>
       </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D42">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
         <v>45040.5</v>
       </c>
@@ -7260,8 +5849,11 @@
       <c r="C43">
         <v>14.19</v>
       </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D43">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
         <v>45040.708333333336</v>
       </c>
@@ -7271,8 +5863,11 @@
       <c r="C44">
         <v>14.74</v>
       </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D44">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
         <v>45040.916666666664</v>
       </c>
@@ -7282,8 +5877,11 @@
       <c r="C45">
         <v>18.95</v>
       </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D45">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
         <v>45041.125</v>
       </c>
@@ -7293,8 +5891,11 @@
       <c r="C46">
         <v>26.09</v>
       </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D46">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" s="1">
         <v>45041.333333333336</v>
       </c>
@@ -7304,8 +5905,11 @@
       <c r="C47">
         <v>7.27</v>
       </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D47">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" s="1">
         <v>45041.75</v>
       </c>
@@ -7315,8 +5919,11 @@
       <c r="C48">
         <v>5.33</v>
       </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D48">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" s="1">
         <v>45041.958333333336</v>
       </c>
@@ -7326,8 +5933,11 @@
       <c r="C49">
         <v>5</v>
       </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D49">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" s="1">
         <v>45042.791666666664</v>
       </c>
@@ -7337,8 +5947,11 @@
       <c r="C50">
         <v>12.14</v>
       </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D50">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" s="1">
         <v>45043</v>
       </c>
@@ -7348,8 +5961,11 @@
       <c r="C51">
         <v>10.67</v>
       </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D51">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" s="1">
         <v>45043.208333333336</v>
       </c>
@@ -7359,8 +5975,11 @@
       <c r="C52">
         <v>5.29</v>
       </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D52">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" s="1">
         <v>45043.416666666664</v>
       </c>
@@ -7370,8 +5989,11 @@
       <c r="C53">
         <v>4.12</v>
       </c>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D53">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" s="1">
         <v>45043.625</v>
       </c>
@@ -7381,8 +6003,11 @@
       <c r="C54">
         <v>8.1300000000000008</v>
       </c>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D54">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" s="1">
         <v>45043.833333333336</v>
       </c>
@@ -7392,8 +6017,11 @@
       <c r="C55">
         <v>6.88</v>
       </c>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D55">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" s="1">
         <v>45044.041666666664</v>
       </c>
@@ -7403,8 +6031,11 @@
       <c r="C56">
         <v>4.83</v>
       </c>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D56">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" s="1">
         <v>45044.25</v>
       </c>
@@ -7414,8 +6045,11 @@
       <c r="C57">
         <v>2.35</v>
       </c>
-    </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D57">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" s="1">
         <v>45044.458333333336</v>
       </c>
@@ -7425,8 +6059,11 @@
       <c r="C58">
         <v>5.33</v>
       </c>
-    </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D58">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" s="1">
         <v>45044.666666666664</v>
       </c>
@@ -7436,8 +6073,11 @@
       <c r="C59">
         <v>5.29</v>
       </c>
-    </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D59">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" s="1">
         <v>45044.875</v>
       </c>
@@ -7447,8 +6087,11 @@
       <c r="C60">
         <v>3.23</v>
       </c>
-    </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D60">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" s="1">
         <v>45045.291666666664</v>
       </c>
@@ -7458,8 +6101,11 @@
       <c r="C61">
         <v>3.33</v>
       </c>
-    </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D61">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" s="1">
         <v>45045.5</v>
       </c>
@@ -7469,8 +6115,11 @@
       <c r="C62">
         <v>5.33</v>
       </c>
-    </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D62">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" s="1">
         <v>45045.916666666664</v>
       </c>
@@ -7480,8 +6129,11 @@
       <c r="C63">
         <v>10.67</v>
       </c>
-    </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D63">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" s="1">
         <v>45046.125</v>
       </c>
@@ -7491,8 +6143,11 @@
       <c r="C64">
         <v>7.86</v>
       </c>
-    </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D64">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" s="1">
         <v>45046.333333333336</v>
       </c>
@@ -7502,8 +6157,11 @@
       <c r="C65">
         <v>8.67</v>
       </c>
-    </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D65">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" s="1">
         <v>45046.541666666664</v>
       </c>
@@ -7513,20 +6171,20 @@
       <c r="C66">
         <v>9.3800000000000008</v>
       </c>
-    </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D66">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" s="2">
         <v>45046.75</v>
       </c>
       <c r="C67" s="3"/>
-      <c r="D67" s="3">
-        <v>63.186318</v>
-      </c>
-      <c r="E67">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D67">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" s="1">
         <v>45046.958333333336</v>
       </c>
@@ -7536,8 +6194,11 @@
       <c r="C68">
         <v>17.420000000000002</v>
       </c>
-    </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D68">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" s="1">
         <v>45047.166666666664</v>
       </c>
@@ -7547,8 +6208,11 @@
       <c r="C69">
         <v>6.67</v>
       </c>
-    </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D69">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" s="1">
         <v>45047.375</v>
       </c>
@@ -7558,8 +6222,11 @@
       <c r="C70">
         <v>2.5</v>
       </c>
-    </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D70">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" s="1">
         <v>45047.583333333336</v>
       </c>
@@ -7569,8 +6236,11 @@
       <c r="C71">
         <v>6</v>
       </c>
-    </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D71">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" s="1">
         <v>45047.833333333336</v>
       </c>
@@ -7580,8 +6250,11 @@
       <c r="C72">
         <v>22.14</v>
       </c>
-    </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D72">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" s="1">
         <v>45048.125</v>
       </c>
@@ -7591,8 +6264,11 @@
       <c r="C73">
         <v>10</v>
       </c>
-    </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D73">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" s="1">
         <v>45048.416666666664</v>
       </c>
@@ -7602,8 +6278,11 @@
       <c r="C74">
         <v>6.43</v>
       </c>
-    </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D74">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75" s="1">
         <v>45048.708333333336</v>
       </c>
@@ -7613,8 +6292,11 @@
       <c r="C75">
         <v>18</v>
       </c>
-    </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D75">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76" s="1">
         <v>45049</v>
       </c>
@@ -7624,8 +6306,11 @@
       <c r="C76">
         <v>9.33</v>
       </c>
-    </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D76">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" s="1">
         <v>45049.291666666664</v>
       </c>
@@ -7635,8 +6320,11 @@
       <c r="C77">
         <v>5.71</v>
       </c>
-    </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D77">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78" s="1">
         <v>45049.583333333336</v>
       </c>
@@ -7646,8 +6334,11 @@
       <c r="C78">
         <v>2.86</v>
       </c>
-    </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D78">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79" s="1">
         <v>45049.833333333336</v>
       </c>
@@ -7657,8 +6348,11 @@
       <c r="C79">
         <v>20.67</v>
       </c>
-    </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D79">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80" s="1">
         <v>45050.083333333336</v>
       </c>
@@ -7667,6 +6361,9 @@
       </c>
       <c r="C80">
         <v>4.67</v>
+      </c>
+      <c r="D80">
+        <v>2</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.25">
@@ -7679,6 +6376,9 @@
       <c r="C81">
         <v>11.88</v>
       </c>
+      <c r="D81">
+        <v>2</v>
+      </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A82" s="1">
@@ -7690,6 +6390,9 @@
       <c r="C82">
         <v>2.86</v>
       </c>
+      <c r="D82">
+        <v>2</v>
+      </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A83" s="1">
@@ -7701,6 +6404,9 @@
       <c r="C83">
         <v>8.75</v>
       </c>
+      <c r="D83">
+        <v>2</v>
+      </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A84" s="2">
@@ -7711,7 +6417,7 @@
       </c>
       <c r="C84" s="3"/>
       <c r="D84">
-        <v>187</v>
+        <v>1</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.25">
@@ -7724,6 +6430,9 @@
       <c r="C85">
         <v>110</v>
       </c>
+      <c r="D85">
+        <v>1</v>
+      </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A86" s="1">
@@ -7735,6 +6444,9 @@
       <c r="C86">
         <v>53.33</v>
       </c>
+      <c r="D86">
+        <v>1</v>
+      </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A87" s="1">
@@ -7746,6 +6458,9 @@
       <c r="C87">
         <v>80</v>
       </c>
+      <c r="D87">
+        <v>1</v>
+      </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A88" s="1">
@@ -7757,6 +6472,9 @@
       <c r="C88">
         <v>43.33</v>
       </c>
+      <c r="D88">
+        <v>1</v>
+      </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A89" s="1">
@@ -7768,6 +6486,9 @@
       <c r="C89">
         <v>92.22</v>
       </c>
+      <c r="D89">
+        <v>1</v>
+      </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A90" s="1">
@@ -7779,6 +6500,9 @@
       <c r="C90">
         <v>52.22</v>
       </c>
+      <c r="D90">
+        <v>1</v>
+      </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A91" s="1">
@@ -7845,8 +6569,11 @@
       <c r="C96">
         <v>37.6</v>
       </c>
-    </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D96">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A97" s="1">
         <v>45183.754861111112</v>
       </c>
@@ -7856,8 +6583,11 @@
       <c r="C97">
         <v>31.54</v>
       </c>
-    </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D97">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A98" s="1">
         <v>45183.765277777777</v>
       </c>
@@ -7867,8 +6597,11 @@
       <c r="C98">
         <v>28.08</v>
       </c>
-    </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D98">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A99" s="1">
         <v>45183.775694444441</v>
       </c>
@@ -7878,8 +6611,11 @@
       <c r="C99">
         <v>23.6</v>
       </c>
-    </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D99">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A100" s="1">
         <v>45183.786111111112</v>
       </c>
@@ -7889,8 +6625,11 @@
       <c r="C100">
         <v>21.18</v>
       </c>
-    </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D100">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A101" s="1">
         <v>45183.79791666667</v>
       </c>
@@ -7899,6 +6638,9 @@
       </c>
       <c r="C101">
         <v>23.14</v>
+      </c>
+      <c r="D101">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>